<commit_message>
Add 1k annotated tweets of session 1
</commit_message>
<xml_diff>
--- a/Datasets/annotated_dataset/tweets_session_1_2.xlsx
+++ b/Datasets/annotated_dataset/tweets_session_1_2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/markusbink/Documents/dev/Twitter_German_Federal_Election_Perception_2021/Datasets/annotated_dataset/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{517968D3-ECCF-6A4F-91BB-87E647BAD0D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A78812CA-FC4B-A846-B5BE-952324162E7C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="35840" windowHeight="21900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6891" uniqueCount="4057">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7007" uniqueCount="4057">
   <si>
     <t>id</t>
   </si>
@@ -12562,8 +12562,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I1001"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A885" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="E886" sqref="E886"/>
+    <sheetView tabSelected="1" topLeftCell="A989" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="E1001" sqref="E1001"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -38247,6 +38247,9 @@
       <c r="D886" t="s">
         <v>3596</v>
       </c>
+      <c r="E886" t="s">
+        <v>4054</v>
+      </c>
       <c r="F886" s="3" t="s">
         <v>3597</v>
       </c>
@@ -38273,6 +38276,9 @@
       <c r="D887" t="s">
         <v>3600</v>
       </c>
+      <c r="E887" t="s">
+        <v>4054</v>
+      </c>
       <c r="F887" s="3" t="s">
         <v>3601</v>
       </c>
@@ -38299,6 +38305,9 @@
       <c r="D888" t="s">
         <v>3604</v>
       </c>
+      <c r="E888" t="s">
+        <v>4054</v>
+      </c>
       <c r="F888" s="3" t="s">
         <v>3605</v>
       </c>
@@ -38325,6 +38334,9 @@
       <c r="D889" t="s">
         <v>3608</v>
       </c>
+      <c r="E889" t="s">
+        <v>4054</v>
+      </c>
       <c r="F889" s="3" t="s">
         <v>3609</v>
       </c>
@@ -38351,6 +38363,9 @@
       <c r="D890" t="s">
         <v>3612</v>
       </c>
+      <c r="E890" t="s">
+        <v>4054</v>
+      </c>
       <c r="F890" s="3" t="s">
         <v>3613</v>
       </c>
@@ -38377,6 +38392,9 @@
       <c r="D891" t="s">
         <v>3616</v>
       </c>
+      <c r="E891" t="s">
+        <v>4056</v>
+      </c>
       <c r="F891" s="3" t="s">
         <v>3617</v>
       </c>
@@ -38403,6 +38421,9 @@
       <c r="D892" t="s">
         <v>3620</v>
       </c>
+      <c r="E892" t="s">
+        <v>4054</v>
+      </c>
       <c r="F892" s="3" t="s">
         <v>3621</v>
       </c>
@@ -38429,6 +38450,9 @@
       <c r="D893" t="s">
         <v>3624</v>
       </c>
+      <c r="E893" t="s">
+        <v>4054</v>
+      </c>
       <c r="F893" s="3" t="s">
         <v>3625</v>
       </c>
@@ -38455,6 +38479,9 @@
       <c r="D894" t="s">
         <v>3628</v>
       </c>
+      <c r="E894" t="s">
+        <v>4054</v>
+      </c>
       <c r="F894" s="3" t="s">
         <v>3629</v>
       </c>
@@ -38481,6 +38508,9 @@
       <c r="D895" t="s">
         <v>3632</v>
       </c>
+      <c r="E895" t="s">
+        <v>4056</v>
+      </c>
       <c r="F895" s="3" t="s">
         <v>3633</v>
       </c>
@@ -38507,6 +38537,9 @@
       <c r="D896" t="s">
         <v>3636</v>
       </c>
+      <c r="E896" t="s">
+        <v>4055</v>
+      </c>
       <c r="F896" s="3" t="s">
         <v>3637</v>
       </c>
@@ -38533,6 +38566,9 @@
       <c r="D897" t="s">
         <v>3640</v>
       </c>
+      <c r="E897" t="s">
+        <v>4056</v>
+      </c>
       <c r="F897" s="3" t="s">
         <v>3641</v>
       </c>
@@ -38559,6 +38595,9 @@
       <c r="D898" t="s">
         <v>3644</v>
       </c>
+      <c r="E898" t="s">
+        <v>4056</v>
+      </c>
       <c r="F898" s="3" t="s">
         <v>3645</v>
       </c>
@@ -38585,6 +38624,9 @@
       <c r="D899" t="s">
         <v>3648</v>
       </c>
+      <c r="E899" t="s">
+        <v>4056</v>
+      </c>
       <c r="F899" s="3" t="s">
         <v>3649</v>
       </c>
@@ -38611,6 +38653,9 @@
       <c r="D900" t="s">
         <v>3652</v>
       </c>
+      <c r="E900" t="s">
+        <v>4056</v>
+      </c>
       <c r="F900" s="3" t="s">
         <v>3653</v>
       </c>
@@ -38637,6 +38682,9 @@
       <c r="D901" t="s">
         <v>3656</v>
       </c>
+      <c r="E901" t="s">
+        <v>4056</v>
+      </c>
       <c r="F901" s="3" t="s">
         <v>3657</v>
       </c>
@@ -38663,6 +38711,9 @@
       <c r="D902" t="s">
         <v>3660</v>
       </c>
+      <c r="E902" t="s">
+        <v>4054</v>
+      </c>
       <c r="F902" s="3" t="s">
         <v>3661</v>
       </c>
@@ -38689,6 +38740,9 @@
       <c r="D903" t="s">
         <v>3664</v>
       </c>
+      <c r="E903" t="s">
+        <v>4054</v>
+      </c>
       <c r="F903" s="3" t="s">
         <v>3665</v>
       </c>
@@ -38715,6 +38769,9 @@
       <c r="D904" t="s">
         <v>3668</v>
       </c>
+      <c r="E904" t="s">
+        <v>4056</v>
+      </c>
       <c r="F904" s="3" t="s">
         <v>3669</v>
       </c>
@@ -38741,6 +38798,9 @@
       <c r="D905" t="s">
         <v>3672</v>
       </c>
+      <c r="E905" t="s">
+        <v>4054</v>
+      </c>
       <c r="F905" s="3" t="s">
         <v>3673</v>
       </c>
@@ -38767,6 +38827,9 @@
       <c r="D906" t="s">
         <v>3676</v>
       </c>
+      <c r="E906" t="s">
+        <v>4053</v>
+      </c>
       <c r="F906" s="3" t="s">
         <v>3677</v>
       </c>
@@ -38793,6 +38856,9 @@
       <c r="D907" t="s">
         <v>3680</v>
       </c>
+      <c r="E907" t="s">
+        <v>4056</v>
+      </c>
       <c r="F907" s="3" t="s">
         <v>3681</v>
       </c>
@@ -38819,6 +38885,9 @@
       <c r="D908" t="s">
         <v>3685</v>
       </c>
+      <c r="E908" t="s">
+        <v>4056</v>
+      </c>
       <c r="F908" s="3" t="s">
         <v>3686</v>
       </c>
@@ -38845,6 +38914,9 @@
       <c r="D909" t="s">
         <v>3689</v>
       </c>
+      <c r="E909" t="s">
+        <v>4056</v>
+      </c>
       <c r="F909" s="3" t="s">
         <v>3690</v>
       </c>
@@ -38871,6 +38943,9 @@
       <c r="D910" t="s">
         <v>3693</v>
       </c>
+      <c r="E910" t="s">
+        <v>4054</v>
+      </c>
       <c r="F910" s="3" t="s">
         <v>3694</v>
       </c>
@@ -38897,6 +38972,9 @@
       <c r="D911" t="s">
         <v>3697</v>
       </c>
+      <c r="E911" t="s">
+        <v>4056</v>
+      </c>
       <c r="F911" s="3" t="s">
         <v>3698</v>
       </c>
@@ -38923,6 +39001,9 @@
       <c r="D912" t="s">
         <v>3701</v>
       </c>
+      <c r="E912" t="s">
+        <v>4054</v>
+      </c>
       <c r="F912" s="3" t="s">
         <v>3702</v>
       </c>
@@ -38949,6 +39030,9 @@
       <c r="D913" t="s">
         <v>3705</v>
       </c>
+      <c r="E913" t="s">
+        <v>4053</v>
+      </c>
       <c r="F913" s="3" t="s">
         <v>3706</v>
       </c>
@@ -38975,6 +39059,9 @@
       <c r="D914" t="s">
         <v>3709</v>
       </c>
+      <c r="E914" t="s">
+        <v>4056</v>
+      </c>
       <c r="F914" s="3" t="s">
         <v>3710</v>
       </c>
@@ -39001,6 +39088,9 @@
       <c r="D915" t="s">
         <v>3713</v>
       </c>
+      <c r="E915" t="s">
+        <v>4056</v>
+      </c>
       <c r="F915" s="3" t="s">
         <v>3714</v>
       </c>
@@ -39027,6 +39117,9 @@
       <c r="D916" t="s">
         <v>3717</v>
       </c>
+      <c r="E916" t="s">
+        <v>4054</v>
+      </c>
       <c r="F916" s="3" t="s">
         <v>3718</v>
       </c>
@@ -39053,6 +39146,9 @@
       <c r="D917" t="s">
         <v>3721</v>
       </c>
+      <c r="E917" t="s">
+        <v>4054</v>
+      </c>
       <c r="F917" s="3" t="s">
         <v>3722</v>
       </c>
@@ -39079,6 +39175,9 @@
       <c r="D918" t="s">
         <v>3725</v>
       </c>
+      <c r="E918" t="s">
+        <v>4054</v>
+      </c>
       <c r="F918" s="3" t="s">
         <v>3726</v>
       </c>
@@ -39105,6 +39204,9 @@
       <c r="D919" t="s">
         <v>3729</v>
       </c>
+      <c r="E919" t="s">
+        <v>4055</v>
+      </c>
       <c r="F919" s="3" t="s">
         <v>3730</v>
       </c>
@@ -39131,6 +39233,9 @@
       <c r="D920" t="s">
         <v>3733</v>
       </c>
+      <c r="E920" t="s">
+        <v>4056</v>
+      </c>
       <c r="F920" s="3" t="s">
         <v>3734</v>
       </c>
@@ -39157,6 +39262,9 @@
       <c r="D921" t="s">
         <v>3737</v>
       </c>
+      <c r="E921" t="s">
+        <v>4056</v>
+      </c>
       <c r="F921" s="3" t="s">
         <v>3738</v>
       </c>
@@ -39183,6 +39291,9 @@
       <c r="D922" t="s">
         <v>3741</v>
       </c>
+      <c r="E922" t="s">
+        <v>4054</v>
+      </c>
       <c r="F922" s="3" t="s">
         <v>3742</v>
       </c>
@@ -39209,6 +39320,9 @@
       <c r="D923" t="s">
         <v>3745</v>
       </c>
+      <c r="E923" t="s">
+        <v>4056</v>
+      </c>
       <c r="F923" s="3" t="s">
         <v>3746</v>
       </c>
@@ -39235,6 +39349,9 @@
       <c r="D924" t="s">
         <v>3749</v>
       </c>
+      <c r="E924" t="s">
+        <v>4056</v>
+      </c>
       <c r="F924" s="3" t="s">
         <v>3750</v>
       </c>
@@ -39261,6 +39378,9 @@
       <c r="D925" t="s">
         <v>3753</v>
       </c>
+      <c r="E925" t="s">
+        <v>4056</v>
+      </c>
       <c r="F925" s="3" t="s">
         <v>3754</v>
       </c>
@@ -39287,6 +39407,9 @@
       <c r="D926" t="s">
         <v>3757</v>
       </c>
+      <c r="E926" t="s">
+        <v>4056</v>
+      </c>
       <c r="F926" s="3" t="s">
         <v>3758</v>
       </c>
@@ -39313,6 +39436,9 @@
       <c r="D927" t="s">
         <v>3761</v>
       </c>
+      <c r="E927" t="s">
+        <v>4054</v>
+      </c>
       <c r="F927" s="3" t="s">
         <v>3762</v>
       </c>
@@ -39339,6 +39465,9 @@
       <c r="D928" t="s">
         <v>3765</v>
       </c>
+      <c r="E928" t="s">
+        <v>4054</v>
+      </c>
       <c r="F928" s="3" t="s">
         <v>3766</v>
       </c>
@@ -39365,6 +39494,9 @@
       <c r="D929" t="s">
         <v>3769</v>
       </c>
+      <c r="E929" t="s">
+        <v>4054</v>
+      </c>
       <c r="F929" s="3" t="s">
         <v>3770</v>
       </c>
@@ -39391,6 +39523,9 @@
       <c r="D930" t="s">
         <v>3773</v>
       </c>
+      <c r="E930" t="s">
+        <v>4056</v>
+      </c>
       <c r="F930" s="3" t="s">
         <v>3774</v>
       </c>
@@ -39417,6 +39552,9 @@
       <c r="D931" t="s">
         <v>3777</v>
       </c>
+      <c r="E931" t="s">
+        <v>4056</v>
+      </c>
       <c r="F931" s="3" t="s">
         <v>3778</v>
       </c>
@@ -39443,6 +39581,9 @@
       <c r="D932" t="s">
         <v>3781</v>
       </c>
+      <c r="E932" t="s">
+        <v>4054</v>
+      </c>
       <c r="F932" s="3" t="s">
         <v>3782</v>
       </c>
@@ -39469,6 +39610,9 @@
       <c r="D933" t="s">
         <v>3785</v>
       </c>
+      <c r="E933" t="s">
+        <v>4054</v>
+      </c>
       <c r="F933" s="3" t="s">
         <v>3786</v>
       </c>
@@ -39495,6 +39639,9 @@
       <c r="D934" t="s">
         <v>3789</v>
       </c>
+      <c r="E934" t="s">
+        <v>4056</v>
+      </c>
       <c r="F934" s="3" t="s">
         <v>3790</v>
       </c>
@@ -39521,6 +39668,9 @@
       <c r="D935" t="s">
         <v>3793</v>
       </c>
+      <c r="E935" t="s">
+        <v>4056</v>
+      </c>
       <c r="F935" s="3" t="s">
         <v>3794</v>
       </c>
@@ -39547,6 +39697,9 @@
       <c r="D936" t="s">
         <v>3797</v>
       </c>
+      <c r="E936" t="s">
+        <v>4056</v>
+      </c>
       <c r="F936" s="3" t="s">
         <v>3798</v>
       </c>
@@ -39573,6 +39726,9 @@
       <c r="D937" t="s">
         <v>3801</v>
       </c>
+      <c r="E937" t="s">
+        <v>4054</v>
+      </c>
       <c r="F937" s="3" t="s">
         <v>3802</v>
       </c>
@@ -39599,6 +39755,9 @@
       <c r="D938" t="s">
         <v>3805</v>
       </c>
+      <c r="E938" t="s">
+        <v>4056</v>
+      </c>
       <c r="F938" s="3" t="s">
         <v>3806</v>
       </c>
@@ -39625,6 +39784,9 @@
       <c r="D939" t="s">
         <v>3809</v>
       </c>
+      <c r="E939" t="s">
+        <v>4054</v>
+      </c>
       <c r="F939" s="3" t="s">
         <v>3810</v>
       </c>
@@ -39651,6 +39813,9 @@
       <c r="D940" t="s">
         <v>3813</v>
       </c>
+      <c r="E940" t="s">
+        <v>4055</v>
+      </c>
       <c r="F940" s="3" t="s">
         <v>3814</v>
       </c>
@@ -39677,6 +39842,9 @@
       <c r="D941" t="s">
         <v>3817</v>
       </c>
+      <c r="E941" t="s">
+        <v>4054</v>
+      </c>
       <c r="F941" s="3" t="s">
         <v>3818</v>
       </c>
@@ -39703,6 +39871,9 @@
       <c r="D942" t="s">
         <v>3821</v>
       </c>
+      <c r="E942" t="s">
+        <v>4054</v>
+      </c>
       <c r="F942" s="3" t="s">
         <v>3822</v>
       </c>
@@ -39729,6 +39900,9 @@
       <c r="D943" t="s">
         <v>3825</v>
       </c>
+      <c r="E943" t="s">
+        <v>4054</v>
+      </c>
       <c r="F943" s="3" t="s">
         <v>3826</v>
       </c>
@@ -39755,6 +39929,9 @@
       <c r="D944" t="s">
         <v>3829</v>
       </c>
+      <c r="E944" t="s">
+        <v>4056</v>
+      </c>
       <c r="F944" s="3" t="s">
         <v>3830</v>
       </c>
@@ -39781,6 +39958,9 @@
       <c r="D945" t="s">
         <v>3833</v>
       </c>
+      <c r="E945" t="s">
+        <v>4056</v>
+      </c>
       <c r="F945" s="3" t="s">
         <v>3834</v>
       </c>
@@ -39807,6 +39987,9 @@
       <c r="D946" t="s">
         <v>3837</v>
       </c>
+      <c r="E946" t="s">
+        <v>4056</v>
+      </c>
       <c r="F946" s="3" t="s">
         <v>3838</v>
       </c>
@@ -39833,6 +40016,9 @@
       <c r="D947" t="s">
         <v>3841</v>
       </c>
+      <c r="E947" t="s">
+        <v>4055</v>
+      </c>
       <c r="F947" s="3" t="s">
         <v>3842</v>
       </c>
@@ -39859,6 +40045,9 @@
       <c r="D948" t="s">
         <v>3845</v>
       </c>
+      <c r="E948" t="s">
+        <v>4056</v>
+      </c>
       <c r="F948" s="3" t="s">
         <v>3846</v>
       </c>
@@ -39885,6 +40074,9 @@
       <c r="D949" t="s">
         <v>3849</v>
       </c>
+      <c r="E949" t="s">
+        <v>4056</v>
+      </c>
       <c r="F949" s="3" t="s">
         <v>3850</v>
       </c>
@@ -39911,6 +40103,9 @@
       <c r="D950" t="s">
         <v>3853</v>
       </c>
+      <c r="E950" t="s">
+        <v>4056</v>
+      </c>
       <c r="F950" s="3" t="s">
         <v>3854</v>
       </c>
@@ -39937,6 +40132,9 @@
       <c r="D951" t="s">
         <v>3857</v>
       </c>
+      <c r="E951" t="s">
+        <v>4054</v>
+      </c>
       <c r="F951" s="3" t="s">
         <v>3858</v>
       </c>
@@ -39963,6 +40161,9 @@
       <c r="D952" t="s">
         <v>3861</v>
       </c>
+      <c r="E952" t="s">
+        <v>4054</v>
+      </c>
       <c r="F952" s="3" t="s">
         <v>3862</v>
       </c>
@@ -39989,6 +40190,9 @@
       <c r="D953" t="s">
         <v>3865</v>
       </c>
+      <c r="E953" t="s">
+        <v>4056</v>
+      </c>
       <c r="F953" s="3" t="s">
         <v>3866</v>
       </c>
@@ -40015,6 +40219,9 @@
       <c r="D954" t="s">
         <v>3869</v>
       </c>
+      <c r="E954" t="s">
+        <v>4055</v>
+      </c>
       <c r="F954" s="3" t="s">
         <v>3870</v>
       </c>
@@ -40041,6 +40248,9 @@
       <c r="D955" t="s">
         <v>3872</v>
       </c>
+      <c r="E955" t="s">
+        <v>4054</v>
+      </c>
       <c r="F955" s="3" t="s">
         <v>3873</v>
       </c>
@@ -40067,6 +40277,9 @@
       <c r="D956" t="s">
         <v>3876</v>
       </c>
+      <c r="E956" t="s">
+        <v>4056</v>
+      </c>
       <c r="F956" s="3" t="s">
         <v>3877</v>
       </c>
@@ -40093,6 +40306,9 @@
       <c r="D957" t="s">
         <v>3880</v>
       </c>
+      <c r="E957" t="s">
+        <v>4053</v>
+      </c>
       <c r="F957" s="3" t="s">
         <v>3881</v>
       </c>
@@ -40119,6 +40335,9 @@
       <c r="D958" t="s">
         <v>3884</v>
       </c>
+      <c r="E958" t="s">
+        <v>4053</v>
+      </c>
       <c r="F958" s="3" t="s">
         <v>3885</v>
       </c>
@@ -40145,6 +40364,9 @@
       <c r="D959" t="s">
         <v>3888</v>
       </c>
+      <c r="E959" t="s">
+        <v>4056</v>
+      </c>
       <c r="F959" s="3" t="s">
         <v>3889</v>
       </c>
@@ -40171,6 +40393,9 @@
       <c r="D960" t="s">
         <v>3892</v>
       </c>
+      <c r="E960" t="s">
+        <v>4056</v>
+      </c>
       <c r="F960" s="3" t="s">
         <v>3893</v>
       </c>
@@ -40197,6 +40422,9 @@
       <c r="D961" t="s">
         <v>3895</v>
       </c>
+      <c r="E961" t="s">
+        <v>4054</v>
+      </c>
       <c r="F961" s="3" t="s">
         <v>3896</v>
       </c>
@@ -40223,6 +40451,9 @@
       <c r="D962" t="s">
         <v>3899</v>
       </c>
+      <c r="E962" t="s">
+        <v>4056</v>
+      </c>
       <c r="F962" s="3" t="s">
         <v>3900</v>
       </c>
@@ -40249,6 +40480,9 @@
       <c r="D963" t="s">
         <v>3903</v>
       </c>
+      <c r="E963" t="s">
+        <v>4054</v>
+      </c>
       <c r="F963" s="3" t="s">
         <v>3904</v>
       </c>
@@ -40275,6 +40509,9 @@
       <c r="D964" t="s">
         <v>3907</v>
       </c>
+      <c r="E964" t="s">
+        <v>4053</v>
+      </c>
       <c r="F964" s="3" t="s">
         <v>3908</v>
       </c>
@@ -40301,6 +40538,9 @@
       <c r="D965" t="s">
         <v>3911</v>
       </c>
+      <c r="E965" t="s">
+        <v>4054</v>
+      </c>
       <c r="F965" s="3" t="s">
         <v>3912</v>
       </c>
@@ -40327,6 +40567,9 @@
       <c r="D966" t="s">
         <v>3915</v>
       </c>
+      <c r="E966" t="s">
+        <v>4056</v>
+      </c>
       <c r="F966" s="3" t="s">
         <v>3916</v>
       </c>
@@ -40353,6 +40596,9 @@
       <c r="D967" t="s">
         <v>3918</v>
       </c>
+      <c r="E967" t="s">
+        <v>4054</v>
+      </c>
       <c r="F967" s="3" t="s">
         <v>3919</v>
       </c>
@@ -40379,6 +40625,9 @@
       <c r="D968" t="s">
         <v>3921</v>
       </c>
+      <c r="E968" t="s">
+        <v>4056</v>
+      </c>
       <c r="F968" s="3" t="s">
         <v>3922</v>
       </c>
@@ -40405,6 +40654,9 @@
       <c r="D969" t="s">
         <v>3925</v>
       </c>
+      <c r="E969" t="s">
+        <v>4054</v>
+      </c>
       <c r="F969" s="3" t="s">
         <v>3926</v>
       </c>
@@ -40431,6 +40683,9 @@
       <c r="D970" t="s">
         <v>3928</v>
       </c>
+      <c r="E970" t="s">
+        <v>4053</v>
+      </c>
       <c r="F970" s="3" t="s">
         <v>3929</v>
       </c>
@@ -40457,6 +40712,9 @@
       <c r="D971" t="s">
         <v>3932</v>
       </c>
+      <c r="E971" t="s">
+        <v>4053</v>
+      </c>
       <c r="F971" s="3" t="s">
         <v>3933</v>
       </c>
@@ -40483,6 +40741,9 @@
       <c r="D972" t="s">
         <v>3936</v>
       </c>
+      <c r="E972" t="s">
+        <v>4056</v>
+      </c>
       <c r="F972" s="3" t="s">
         <v>3937</v>
       </c>
@@ -40509,6 +40770,9 @@
       <c r="D973" t="s">
         <v>3940</v>
       </c>
+      <c r="E973" t="s">
+        <v>4055</v>
+      </c>
       <c r="F973" s="3" t="s">
         <v>3941</v>
       </c>
@@ -40535,6 +40799,9 @@
       <c r="D974" t="s">
         <v>3944</v>
       </c>
+      <c r="E974" t="s">
+        <v>4054</v>
+      </c>
       <c r="F974" s="3" t="s">
         <v>3945</v>
       </c>
@@ -40561,6 +40828,9 @@
       <c r="D975" t="s">
         <v>3948</v>
       </c>
+      <c r="E975" t="s">
+        <v>4054</v>
+      </c>
       <c r="F975" s="3" t="s">
         <v>3949</v>
       </c>
@@ -40587,6 +40857,9 @@
       <c r="D976" t="s">
         <v>3952</v>
       </c>
+      <c r="E976" t="s">
+        <v>4053</v>
+      </c>
       <c r="F976" s="3" t="s">
         <v>3953</v>
       </c>
@@ -40613,6 +40886,9 @@
       <c r="D977" t="s">
         <v>3956</v>
       </c>
+      <c r="E977" t="s">
+        <v>4056</v>
+      </c>
       <c r="F977" s="3" t="s">
         <v>3957</v>
       </c>
@@ -40639,6 +40915,9 @@
       <c r="D978" t="s">
         <v>3960</v>
       </c>
+      <c r="E978" t="s">
+        <v>4053</v>
+      </c>
       <c r="F978" s="3" t="s">
         <v>3961</v>
       </c>
@@ -40665,6 +40944,9 @@
       <c r="D979" t="s">
         <v>3964</v>
       </c>
+      <c r="E979" t="s">
+        <v>4056</v>
+      </c>
       <c r="F979" s="3" t="s">
         <v>3965</v>
       </c>
@@ -40691,6 +40973,9 @@
       <c r="D980" t="s">
         <v>3967</v>
       </c>
+      <c r="E980" t="s">
+        <v>4056</v>
+      </c>
       <c r="F980" s="3" t="s">
         <v>3968</v>
       </c>
@@ -40717,6 +41002,9 @@
       <c r="D981" t="s">
         <v>3971</v>
       </c>
+      <c r="E981" t="s">
+        <v>4056</v>
+      </c>
       <c r="F981" s="3" t="s">
         <v>3972</v>
       </c>
@@ -40743,6 +41031,9 @@
       <c r="D982" t="s">
         <v>3975</v>
       </c>
+      <c r="E982" t="s">
+        <v>4054</v>
+      </c>
       <c r="F982" s="3" t="s">
         <v>3976</v>
       </c>
@@ -40769,6 +41060,9 @@
       <c r="D983" t="s">
         <v>3979</v>
       </c>
+      <c r="E983" t="s">
+        <v>4054</v>
+      </c>
       <c r="F983" s="3" t="s">
         <v>3980</v>
       </c>
@@ -40795,6 +41089,9 @@
       <c r="D984" t="s">
         <v>3983</v>
       </c>
+      <c r="E984" t="s">
+        <v>4054</v>
+      </c>
       <c r="F984" s="3" t="s">
         <v>3984</v>
       </c>
@@ -40821,6 +41118,9 @@
       <c r="D985" t="s">
         <v>3987</v>
       </c>
+      <c r="E985" t="s">
+        <v>4054</v>
+      </c>
       <c r="F985" s="3" t="s">
         <v>3988</v>
       </c>
@@ -40847,6 +41147,9 @@
       <c r="D986" t="s">
         <v>3991</v>
       </c>
+      <c r="E986" t="s">
+        <v>4054</v>
+      </c>
       <c r="F986" s="3" t="s">
         <v>3992</v>
       </c>
@@ -40873,6 +41176,9 @@
       <c r="D987" t="s">
         <v>3995</v>
       </c>
+      <c r="E987" t="s">
+        <v>4054</v>
+      </c>
       <c r="F987" s="3" t="s">
         <v>3996</v>
       </c>
@@ -40899,6 +41205,9 @@
       <c r="D988" t="s">
         <v>3999</v>
       </c>
+      <c r="E988" t="s">
+        <v>4054</v>
+      </c>
       <c r="F988" s="3" t="s">
         <v>4000</v>
       </c>
@@ -40925,6 +41234,9 @@
       <c r="D989" t="s">
         <v>4003</v>
       </c>
+      <c r="E989" t="s">
+        <v>4053</v>
+      </c>
       <c r="F989" s="3" t="s">
         <v>4004</v>
       </c>
@@ -40951,6 +41263,9 @@
       <c r="D990" t="s">
         <v>4007</v>
       </c>
+      <c r="E990" t="s">
+        <v>4056</v>
+      </c>
       <c r="F990" s="3" t="s">
         <v>4008</v>
       </c>
@@ -40977,6 +41292,9 @@
       <c r="D991" t="s">
         <v>4011</v>
       </c>
+      <c r="E991" t="s">
+        <v>4056</v>
+      </c>
       <c r="F991" s="3" t="s">
         <v>4012</v>
       </c>
@@ -41003,6 +41321,9 @@
       <c r="D992" t="s">
         <v>4015</v>
       </c>
+      <c r="E992" t="s">
+        <v>4053</v>
+      </c>
       <c r="F992" s="3" t="s">
         <v>4016</v>
       </c>
@@ -41029,6 +41350,9 @@
       <c r="D993" t="s">
         <v>4018</v>
       </c>
+      <c r="E993" t="s">
+        <v>4054</v>
+      </c>
       <c r="F993" s="3" t="s">
         <v>4019</v>
       </c>
@@ -41055,6 +41379,9 @@
       <c r="D994" t="s">
         <v>4022</v>
       </c>
+      <c r="E994" t="s">
+        <v>4053</v>
+      </c>
       <c r="F994" s="3" t="s">
         <v>4023</v>
       </c>
@@ -41081,6 +41408,9 @@
       <c r="D995" t="s">
         <v>4026</v>
       </c>
+      <c r="E995" t="s">
+        <v>4054</v>
+      </c>
       <c r="F995" s="3" t="s">
         <v>4027</v>
       </c>
@@ -41107,6 +41437,9 @@
       <c r="D996" t="s">
         <v>4030</v>
       </c>
+      <c r="E996" t="s">
+        <v>4056</v>
+      </c>
       <c r="F996" s="3" t="s">
         <v>4031</v>
       </c>
@@ -41133,6 +41466,9 @@
       <c r="D997" t="s">
         <v>4034</v>
       </c>
+      <c r="E997" t="s">
+        <v>4056</v>
+      </c>
       <c r="F997" s="3" t="s">
         <v>4035</v>
       </c>
@@ -41159,6 +41495,9 @@
       <c r="D998" t="s">
         <v>4038</v>
       </c>
+      <c r="E998" t="s">
+        <v>4056</v>
+      </c>
       <c r="F998" s="3" t="s">
         <v>4039</v>
       </c>
@@ -41185,6 +41524,9 @@
       <c r="D999" t="s">
         <v>4042</v>
       </c>
+      <c r="E999" t="s">
+        <v>4056</v>
+      </c>
       <c r="F999" s="3" t="s">
         <v>4043</v>
       </c>
@@ -41211,6 +41553,9 @@
       <c r="D1000" t="s">
         <v>4046</v>
       </c>
+      <c r="E1000" t="s">
+        <v>4056</v>
+      </c>
       <c r="F1000" s="3" t="s">
         <v>4047</v>
       </c>
@@ -41236,6 +41581,9 @@
       </c>
       <c r="D1001" t="s">
         <v>4050</v>
+      </c>
+      <c r="E1001" t="s">
+        <v>4056</v>
       </c>
       <c r="F1001" s="3" t="s">
         <v>4051</v>

</xml_diff>